<commit_message>
Updated - Pravash Test Line MarkDown
</commit_message>
<xml_diff>
--- a/site/autogen-demo-test/test.xlsx
+++ b/site/autogen-demo-test/test.xlsx
@@ -2,15 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-22.04\home\akasmajhi\source\learning\ai\microsoft\autogen\site\autogen-demo-test\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\prava\source\pc_omniparser\site\autogen-demo-test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B283BA9C-E9B2-4B2E-B53D-2E0087204527}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBD1FBFF-5066-48D8-987F-476779C5FC6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="11625" xr2:uid="{AFDCDE0B-802D-46F9-8C98-14BEB1EEDE14}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11475" xr2:uid="{AFDCDE0B-802D-46F9-8C98-14BEB1EEDE14}"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
@@ -27,8 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -36,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="24">
   <si>
     <t>TC Name</t>
   </si>
@@ -115,6 +113,12 @@
   </si>
   <si>
     <t>This is our T2 - Scenario 4</t>
+  </si>
+  <si>
+    <t>Pravash Test</t>
+  </si>
+  <si>
+    <t>Next Step</t>
   </si>
 </sst>
 </file>
@@ -180,13 +184,13 @@
   </cellStyles>
   <dxfs count="2">
     <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <font>
         <b/>
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -202,12 +206,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{97CDF4E2-0026-4CBB-A1EE-DE8FFB64ABDB}" name="Table1" displayName="Table1" ref="A1:D6" totalsRowShown="0" headerRowDxfId="0">
-  <autoFilter ref="A1:D6" xr:uid="{97CDF4E2-0026-4CBB-A1EE-DE8FFB64ABDB}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{97CDF4E2-0026-4CBB-A1EE-DE8FFB64ABDB}" name="Table1" displayName="Table1" ref="A1:D7" totalsRowShown="0" headerRowDxfId="1">
+  <autoFilter ref="A1:D7" xr:uid="{97CDF4E2-0026-4CBB-A1EE-DE8FFB64ABDB}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{3D791E04-03AC-4C83-AA96-608EA5947C73}" name="Category"/>
     <tableColumn id="2" xr3:uid="{95A80CB8-98E1-47C8-BF29-6B33489C989B}" name="TC Name"/>
-    <tableColumn id="3" xr3:uid="{6A7D25D5-4580-41E2-AD82-CE0021F5A635}" name="How to simulate?" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{6A7D25D5-4580-41E2-AD82-CE0021F5A635}" name="How to simulate?" dataDxfId="0"/>
     <tableColumn id="4" xr3:uid="{3D7534BB-1C22-41B6-BDD4-2C70D4FD5CEF}" name="Implementatin Details"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight20" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -531,10 +535,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78ABD448-7717-4D23-A40B-66425E555E29}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -629,6 +633,20 @@
         <v>21</v>
       </c>
     </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" t="s">
+        <v>23</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>